<commit_message>
Changes to part1.py and Updated README.md
</commit_message>
<xml_diff>
--- a/parameter_iterations.xlsx
+++ b/parameter_iterations.xlsx
@@ -37,69 +37,69 @@
     <t>r2</t>
   </si>
   <si>
-    <t>[131.32796881 -17.02696644  -1.35909671  -6.83141693   3.07230092
- -13.74339922]</t>
-  </si>
-  <si>
-    <t>[134.47836131 -24.87487646  -8.07870334  -9.48337814   3.72777599
-  -9.84893936]</t>
-  </si>
-  <si>
-    <t>[125.79895176  -5.53071625   5.09318266  -2.09039958   2.69530733
- -12.71698988]</t>
-  </si>
-  <si>
-    <t>[134.19805812 -24.31552049  -7.27851311  -9.21794796   3.66587391
- -10.47693436]</t>
-  </si>
-  <si>
-    <t>[101.23583185   8.30704806  19.14939465  19.21142989  14.27882449
-   4.53041392]</t>
-  </si>
-  <si>
-    <t>[125.79119072  -5.52701889   5.09780385  -2.08247931   2.69722679
- -12.70916395]</t>
-  </si>
-  <si>
-    <t>[131.32293575 -17.01530105  -1.35455875  -6.82731733   3.07191386
- -13.74057351]</t>
-  </si>
-  <si>
-    <t>[133.04179195 -21.57721922  -4.49379556  -8.2096937    3.41150335
- -12.35582722]</t>
-  </si>
-  <si>
-    <t>[91.70986427  9.53484058 21.81896253 25.29501381 23.70681754  9.52183636]</t>
-  </si>
-  <si>
-    <t>[116.41404912   3.36118213  12.07858692   6.76406989   4.61316181
-  -5.92284204]</t>
-  </si>
-  <si>
-    <t>[125.79022041  -5.52655707   5.09838135  -2.08148934   2.69746736
- -12.70818589]</t>
-  </si>
-  <si>
-    <t>[132.22634957 -19.42636317  -2.88817052  -7.54688743   3.24124134
- -13.18021062]</t>
-  </si>
-  <si>
-    <t>[64.74702239  8.12477024 18.70658407 24.10148454 28.1194978  10.7840208 ]</t>
-  </si>
-  <si>
-    <t>[91.70733743  9.53462128 21.81860789 25.29508052 23.70948436  9.52191837]</t>
-  </si>
-  <si>
-    <t>[101.23086216   8.30658663  19.14955361  19.21332154  14.2862444
-   4.53181315]</t>
-  </si>
-  <si>
-    <t>[125.78944413  -5.52618767   5.09884334  -2.08069737   2.69765992
- -12.70740348]</t>
-  </si>
-  <si>
-    <t>[128.93556354 -11.23731309   1.86677041  -4.87421255   2.76630884
- -13.97140979]</t>
+    <t>[131.2364964  -16.64550883  -1.0060594   -6.93070061   3.19816635
+ -14.03974108]</t>
+  </si>
+  <si>
+    <t>[134.24591005 -24.07823761  -7.21059431  -9.3614787    3.71753165
+ -10.61433221]</t>
+  </si>
+  <si>
+    <t>[125.63919692  -5.21025143   5.28734973  -2.3325739    3.08494045
+ -12.84449814]</t>
+  </si>
+  <si>
+    <t>[133.97099504 -23.52353407  -6.44941206  -9.1095778    3.66308831
+ -11.19442363]</t>
+  </si>
+  <si>
+    <t>[100.85912181   8.66554549  19.17127601  18.99152721  15.06089239
+   4.62815946]</t>
+  </si>
+  <si>
+    <t>[125.6312466   -5.20642198   5.29193156  -2.3246551    3.08719394
+ -12.836638  ]</t>
+  </si>
+  <si>
+    <t>[131.2313411  -16.63374504  -1.00153965  -6.92671014   3.19803213
+ -14.03686787]</t>
+  </si>
+  <si>
+    <t>[132.83855273 -20.83842695  -3.82691275  -8.16203533   3.44941257
+ -12.88405101]</t>
+  </si>
+  <si>
+    <t>[91.4451399   9.82705427 21.80287556 25.16101307 24.25295063  9.62829275]</t>
+  </si>
+  <si>
+    <t>[116.08518511   3.74223728  12.16790057   6.45839627   5.36125013
+  -5.93210135]</t>
+  </si>
+  <si>
+    <t>[125.63025266  -5.20594368   5.29250415  -2.32366529   3.0874762
+ -12.83565566]</t>
+  </si>
+  <si>
+    <t>[132.03824878 -18.75091543  -2.31946858  -7.5405963    3.31426241
+ -13.60045982]</t>
+  </si>
+  <si>
+    <t>[64.69704467  8.28576561 18.65178557 24.068985   28.26331996 10.83716718]</t>
+  </si>
+  <si>
+    <t>[91.44268645  9.82680798 21.80250519 25.16109714 24.25549534  9.62834432]</t>
+  </si>
+  <si>
+    <t>[100.85431527   8.66501434  19.17141302  18.99348087  15.06800687
+   4.62951743]</t>
+  </si>
+  <si>
+    <t>[125.62945747  -5.2055611    5.29296221  -2.32287345   3.0877021
+ -12.83486982]</t>
+  </si>
+  <si>
+    <t>[128.78318708 -10.82260412   2.17994392  -5.01267959   3.00126881
+ -14.16043813]</t>
   </si>
 </sst>
 </file>
@@ -497,16 +497,16 @@
         <v>7</v>
       </c>
       <c r="D2">
-        <v>24.19010254535689</v>
+        <v>25.81123860303021</v>
       </c>
       <c r="E2">
-        <v>3.996276951927682</v>
+        <v>4.039592301893429</v>
       </c>
       <c r="F2">
-        <v>4.918343475740271</v>
+        <v>5.080476218134498</v>
       </c>
       <c r="G2">
-        <v>0.4927326310085249</v>
+        <v>0.4432657925703599</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -514,22 +514,22 @@
         <v>0.1</v>
       </c>
       <c r="B3">
-        <v>2448</v>
+        <v>2365</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>
       <c r="D3">
-        <v>22.56736907885033</v>
+        <v>22.7884037955823</v>
       </c>
       <c r="E3">
-        <v>3.703931285288628</v>
+        <v>3.687374475178071</v>
       </c>
       <c r="F3">
-        <v>4.750512506967046</v>
+        <v>4.77372012120341</v>
       </c>
       <c r="G3">
-        <v>0.5267614134242158</v>
+        <v>0.508466675278781</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -537,22 +537,22 @@
         <v>0.1</v>
       </c>
       <c r="B4">
-        <v>2448</v>
+        <v>2365</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
       <c r="D4">
-        <v>22.56736907885033</v>
+        <v>22.7884037955823</v>
       </c>
       <c r="E4">
-        <v>3.703931285288628</v>
+        <v>3.687374475178071</v>
       </c>
       <c r="F4">
-        <v>4.750512506967046</v>
+        <v>4.77372012120341</v>
       </c>
       <c r="G4">
-        <v>0.5267614134242158</v>
+        <v>0.508466675278781</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -560,22 +560,22 @@
         <v>0.1</v>
       </c>
       <c r="B5">
-        <v>2448</v>
+        <v>2365</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
       <c r="D5">
-        <v>22.56736907885033</v>
+        <v>22.7884037955823</v>
       </c>
       <c r="E5">
-        <v>3.703931285288628</v>
+        <v>3.687374475178071</v>
       </c>
       <c r="F5">
-        <v>4.750512506967046</v>
+        <v>4.77372012120341</v>
       </c>
       <c r="G5">
-        <v>0.5267614134242158</v>
+        <v>0.508466675278781</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -583,22 +583,22 @@
         <v>0.1</v>
       </c>
       <c r="B6">
-        <v>2448</v>
+        <v>2365</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
       <c r="D6">
-        <v>22.56736907885033</v>
+        <v>22.7884037955823</v>
       </c>
       <c r="E6">
-        <v>3.703931285288628</v>
+        <v>3.687374475178071</v>
       </c>
       <c r="F6">
-        <v>4.750512506967046</v>
+        <v>4.77372012120341</v>
       </c>
       <c r="G6">
-        <v>0.5267614134242158</v>
+        <v>0.508466675278781</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -612,16 +612,16 @@
         <v>9</v>
       </c>
       <c r="D7">
-        <v>33.86112289021799</v>
+        <v>36.20672385672024</v>
       </c>
       <c r="E7">
-        <v>4.851875004658926</v>
+        <v>4.894971754062493</v>
       </c>
       <c r="F7">
-        <v>5.819031095484711</v>
+        <v>6.017202328052484</v>
       </c>
       <c r="G7">
-        <v>0.2899309671213105</v>
+        <v>0.2190408984236615</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -629,22 +629,22 @@
         <v>0.05</v>
       </c>
       <c r="B8">
-        <v>4248</v>
+        <v>4112</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
       </c>
       <c r="D8">
-        <v>22.53347228462743</v>
+        <v>22.94256288127496</v>
       </c>
       <c r="E8">
-        <v>3.709549926523648</v>
+        <v>3.70846947769063</v>
       </c>
       <c r="F8">
-        <v>4.746943467603909</v>
+        <v>4.789839546506225</v>
       </c>
       <c r="G8">
-        <v>0.5274722304862954</v>
+        <v>0.5051415486658681</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -652,22 +652,22 @@
         <v>0.05</v>
       </c>
       <c r="B9">
-        <v>4248</v>
+        <v>4112</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
       </c>
       <c r="D9">
-        <v>22.53347228462743</v>
+        <v>22.94256288127496</v>
       </c>
       <c r="E9">
-        <v>3.709549926523648</v>
+        <v>3.70846947769063</v>
       </c>
       <c r="F9">
-        <v>4.746943467603909</v>
+        <v>4.789839546506225</v>
       </c>
       <c r="G9">
-        <v>0.5274722304862954</v>
+        <v>0.5051415486658681</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -675,22 +675,22 @@
         <v>0.05</v>
       </c>
       <c r="B10">
-        <v>4248</v>
+        <v>4112</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
       </c>
       <c r="D10">
-        <v>22.53347228462743</v>
+        <v>22.94256288127496</v>
       </c>
       <c r="E10">
-        <v>3.709549926523648</v>
+        <v>3.70846947769063</v>
       </c>
       <c r="F10">
-        <v>4.746943467603909</v>
+        <v>4.789839546506225</v>
       </c>
       <c r="G10">
-        <v>0.5274722304862954</v>
+        <v>0.5051415486658681</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -698,22 +698,22 @@
         <v>0.05</v>
       </c>
       <c r="B11">
-        <v>4248</v>
+        <v>4112</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
       </c>
       <c r="D11">
-        <v>22.53347228462743</v>
+        <v>22.94256288127496</v>
       </c>
       <c r="E11">
-        <v>3.709549926523648</v>
+        <v>3.70846947769063</v>
       </c>
       <c r="F11">
-        <v>4.746943467603909</v>
+        <v>4.789839546506225</v>
       </c>
       <c r="G11">
-        <v>0.5274722304862954</v>
+        <v>0.5051415486658681</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -727,16 +727,16 @@
         <v>11</v>
       </c>
       <c r="D12">
-        <v>147.2249759027425</v>
+        <v>161.000942040299</v>
       </c>
       <c r="E12">
-        <v>9.739178987869417</v>
+        <v>10.07335377763749</v>
       </c>
       <c r="F12">
-        <v>12.13362995573635</v>
+        <v>12.68861466198335</v>
       </c>
       <c r="G12">
-        <v>-2.087313335525824</v>
+        <v>-2.472701687849581</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -750,16 +750,16 @@
         <v>12</v>
       </c>
       <c r="D13">
-        <v>33.87204928351608</v>
+        <v>36.21752080781211</v>
       </c>
       <c r="E13">
-        <v>4.852594726159288</v>
+        <v>4.895540799691773</v>
       </c>
       <c r="F13">
-        <v>5.819969869639884</v>
+        <v>6.018099434855834</v>
       </c>
       <c r="G13">
-        <v>0.2897018402389213</v>
+        <v>0.2188080141323946</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -773,16 +773,16 @@
         <v>13</v>
       </c>
       <c r="D14">
-        <v>24.19443261686871</v>
+        <v>25.81649876321331</v>
       </c>
       <c r="E14">
-        <v>3.996846262547968</v>
+        <v>4.040263705108595</v>
       </c>
       <c r="F14">
-        <v>4.91878365217141</v>
+        <v>5.08099387553393</v>
       </c>
       <c r="G14">
-        <v>0.4926418292444882</v>
+        <v>0.4431523338109595</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -790,22 +790,22 @@
         <v>0.01</v>
       </c>
       <c r="B15">
-        <v>14439</v>
+        <v>14091</v>
       </c>
       <c r="C15" t="s">
         <v>14</v>
       </c>
       <c r="D15">
-        <v>22.78476344283738</v>
+        <v>23.8517360346627</v>
       </c>
       <c r="E15">
-        <v>3.794062801695114</v>
+        <v>3.817906185694159</v>
       </c>
       <c r="F15">
-        <v>4.773338815005424</v>
+        <v>4.883823915198284</v>
       </c>
       <c r="G15">
-        <v>0.5222026453558904</v>
+        <v>0.4855311842524297</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -813,22 +813,22 @@
         <v>0.01</v>
       </c>
       <c r="B16">
-        <v>14439</v>
+        <v>14091</v>
       </c>
       <c r="C16" t="s">
         <v>14</v>
       </c>
       <c r="D16">
-        <v>22.78476344283738</v>
+        <v>23.8517360346627</v>
       </c>
       <c r="E16">
-        <v>3.794062801695114</v>
+        <v>3.817906185694159</v>
       </c>
       <c r="F16">
-        <v>4.773338815005424</v>
+        <v>4.883823915198284</v>
       </c>
       <c r="G16">
-        <v>0.5222026453558904</v>
+        <v>0.4855311842524297</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -842,16 +842,16 @@
         <v>15</v>
       </c>
       <c r="D17">
-        <v>238.5995855303832</v>
+        <v>265.4033102641184</v>
       </c>
       <c r="E17">
-        <v>12.28633682326245</v>
+        <v>12.9718907269005</v>
       </c>
       <c r="F17">
-        <v>15.44666907557688</v>
+        <v>16.29120346273161</v>
       </c>
       <c r="G17">
-        <v>-4.003442369353885</v>
+        <v>-4.724603296323409</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -865,16 +865,16 @@
         <v>16</v>
       </c>
       <c r="D18">
-        <v>61.95937953125102</v>
+        <v>65.18339914766948</v>
       </c>
       <c r="E18">
-        <v>6.394514960833965</v>
+        <v>6.419307981178758</v>
       </c>
       <c r="F18">
-        <v>7.871428049042373</v>
+        <v>8.07362366894008</v>
       </c>
       <c r="G18">
-        <v>-0.2992905416680305</v>
+        <v>-0.4059700357729927</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -888,16 +888,16 @@
         <v>17</v>
       </c>
       <c r="D19">
-        <v>33.87341591049874</v>
+        <v>36.21887157205011</v>
       </c>
       <c r="E19">
-        <v>4.852684641050016</v>
+        <v>4.895615246242927</v>
       </c>
       <c r="F19">
-        <v>5.820087276879852</v>
+        <v>6.018211658960667</v>
       </c>
       <c r="G19">
-        <v>0.2896731820191978</v>
+        <v>0.2187788788913845</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -905,22 +905,22 @@
         <v>0.005</v>
       </c>
       <c r="B20">
-        <v>23836</v>
+        <v>23378</v>
       </c>
       <c r="C20" t="s">
         <v>18</v>
       </c>
       <c r="D20">
-        <v>23.31064988280269</v>
+        <v>24.74048473864464</v>
       </c>
       <c r="E20">
-        <v>3.877284251971415</v>
+        <v>3.916503232068693</v>
       </c>
       <c r="F20">
-        <v>4.828110384281069</v>
+        <v>4.973980773851528</v>
       </c>
       <c r="G20">
-        <v>0.511174786739363</v>
+        <v>0.4663613639688957</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -928,22 +928,22 @@
         <v>0.005</v>
       </c>
       <c r="B21">
-        <v>23836</v>
+        <v>23378</v>
       </c>
       <c r="C21" t="s">
         <v>18</v>
       </c>
       <c r="D21">
-        <v>23.31064988280269</v>
+        <v>24.74048473864464</v>
       </c>
       <c r="E21">
-        <v>3.877284251971415</v>
+        <v>3.916503232068693</v>
       </c>
       <c r="F21">
-        <v>4.828110384281069</v>
+        <v>4.973980773851528</v>
       </c>
       <c r="G21">
-        <v>0.511174786739363</v>
+        <v>0.4663613639688957</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -957,16 +957,16 @@
         <v>19</v>
       </c>
       <c r="D22">
-        <v>945.4124619914235</v>
+        <v>982.4970966763094</v>
       </c>
       <c r="E22">
-        <v>26.92370128052619</v>
+        <v>27.29431325941375</v>
       </c>
       <c r="F22">
-        <v>30.74756026079831</v>
+        <v>31.34480972467865</v>
       </c>
       <c r="G22">
-        <v>-18.82533522984976</v>
+        <v>-20.19192150491343</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -980,16 +980,16 @@
         <v>20</v>
       </c>
       <c r="D23">
-        <v>238.6168015460976</v>
+        <v>265.4239058537672</v>
       </c>
       <c r="E23">
-        <v>12.2868409793729</v>
+        <v>12.97243130745867</v>
       </c>
       <c r="F23">
-        <v>15.4472263382815</v>
+        <v>16.29183555814897</v>
       </c>
       <c r="G23">
-        <v>-4.003803389857191</v>
+        <v>-4.725047531854142</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1003,16 +1003,16 @@
         <v>21</v>
       </c>
       <c r="D24">
-        <v>147.2610559377769</v>
+        <v>161.0459211761516</v>
       </c>
       <c r="E24">
-        <v>9.740302609525502</v>
+        <v>10.07478284641877</v>
       </c>
       <c r="F24">
-        <v>12.13511664294072</v>
+        <v>12.69038695927558</v>
       </c>
       <c r="G24">
-        <v>-2.08806993523063</v>
+        <v>-2.473671863048645</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1026,16 +1026,16 @@
         <v>22</v>
       </c>
       <c r="D25">
-        <v>33.87450934449642</v>
+        <v>36.21995236675074</v>
       </c>
       <c r="E25">
-        <v>4.852756564910965</v>
+        <v>4.895674800885466</v>
       </c>
       <c r="F25">
-        <v>5.820181212341796</v>
+        <v>6.018301451967219</v>
       </c>
       <c r="G25">
-        <v>0.2896502526667434</v>
+        <v>0.2187555667446756</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1043,22 +1043,22 @@
         <v>0.001</v>
       </c>
       <c r="B26">
-        <v>70105</v>
+        <v>69719</v>
       </c>
       <c r="C26" t="s">
         <v>23</v>
       </c>
       <c r="D26">
-        <v>27.67147426957951</v>
+        <v>29.86487823079107</v>
       </c>
       <c r="E26">
-        <v>4.371828589838842</v>
+        <v>4.44180804949558</v>
       </c>
       <c r="F26">
-        <v>5.260368263684541</v>
+        <v>5.464876780933956</v>
       </c>
       <c r="G26">
-        <v>0.4197281337470327</v>
+        <v>0.3558310173518673</v>
       </c>
     </row>
   </sheetData>

</xml_diff>